<commit_message>
Versión final post Corrección de estilo
</commit_message>
<xml_diff>
--- a/fuentes/contenidos/grado05/guion05/SolicitudGrafica_LE_05_05.xlsx
+++ b/fuentes/contenidos/grado05/guion05/SolicitudGrafica_LE_05_05.xlsx
@@ -2336,7 +2336,7 @@
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="120" workbookViewId="0">
       <pane ySplit="9" topLeftCell="A15" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E5" sqref="E5"/>
+      <selection pane="bottomLeft" activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="13" x14ac:dyDescent="0"/>
@@ -2395,7 +2395,9 @@
         <v>5</v>
       </c>
       <c r="D3" s="89"/>
-      <c r="F3" s="81"/>
+      <c r="F3" s="81">
+        <v>42087</v>
+      </c>
       <c r="G3" s="82"/>
       <c r="H3" s="56"/>
       <c r="I3" s="56"/>

</xml_diff>